<commit_message>
chore: atualizar base de medições
</commit_message>
<xml_diff>
--- a/AUXILIAR.xlsx
+++ b/AUXILIAR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\APRENDIZADO APP\MEDIÇÕES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9619EB45-BD40-4774-9F4D-E0CC9353538B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8727B70-ABAA-437A-9190-69A5C2B0BC94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C423DC18-ADE7-4847-83C1-B9A17E509C00}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C423DC18-ADE7-4847-83C1-B9A17E509C00}"/>
   </bookViews>
   <sheets>
     <sheet name="AUXILIAR" sheetId="1" r:id="rId1"/>
@@ -1655,8 +1655,8 @@
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{36ACF105-7C04-4C2F-BBBB-C0D7709C893E}" name="CONCLUIDAS" displayName="CONCLUIDAS" ref="M1:N20" totalsRowShown="0">
   <autoFilter ref="M1:N20" xr:uid="{2C0FD495-D559-4428-9974-93B6DDD5F730}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M2:N19">
-    <sortCondition ref="M1:M19"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M2:N20">
+    <sortCondition ref="M1:M20"/>
   </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{BF27031E-8748-4BA6-8E8A-2457B029F7AB}" name="SEI" dataDxfId="1"/>

</xml_diff>

<commit_message>
refactor: Adjust Excel column width calculations for money, date, and various specific contract-related fields.
</commit_message>
<xml_diff>
--- a/AUXILIAR.xlsx
+++ b/AUXILIAR.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\APRENDIZADO APP\MEDIÇÕES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\APRENDIZADO APP\MEDICOES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8727B70-ABAA-437A-9190-69A5C2B0BC94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3CFC553-6EC1-4797-AC79-9404664903C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C423DC18-ADE7-4847-83C1-B9A17E509C00}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="356">
   <si>
     <t>NORTE</t>
   </si>
@@ -1106,12 +1106,15 @@
   </si>
   <si>
     <t>TANGRAN ENGENHARIA</t>
+  </si>
+  <si>
+    <t>SOLVE CONSULTORIA E PROJETOS LTDA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1574,7 +1577,9 @@
       </border>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{3CFF4B64-F1B6-4152-AC6B-5BFD73E20E31}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1639,10 +1644,10 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0B7CAE8F-BE59-4435-A0C5-FB4478B9C026}" name="Contratadas" displayName="Contratadas" ref="J1:K121" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="J1:K121" xr:uid="{580F5E59-D6E0-45CB-9D08-B88FBCDB53A2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="J2:K121">
-    <sortCondition ref="J1:J121"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0B7CAE8F-BE59-4435-A0C5-FB4478B9C026}" name="Contratadas" displayName="Contratadas" ref="J1:K122" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="J1:K122" xr:uid="{580F5E59-D6E0-45CB-9D08-B88FBCDB53A2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="J2:K122">
+    <sortCondition ref="J1:J122"/>
   </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{34535A94-5211-4138-9717-46CE0AA9504A}" name="CONTRATADA"/>
@@ -1984,10 +1989,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF6E23BC-EFB1-49F0-A739-0222D98A9D41}">
   <sheetPr codeName="Planilha3"/>
-  <dimension ref="B1:N121"/>
+  <dimension ref="B1:N122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView tabSelected="1" topLeftCell="D88" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="K65" sqref="K65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2369,10 +2374,10 @@
         <v>104</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>105</v>
+        <v>353</v>
       </c>
       <c r="K16" s="7" t="s">
-        <v>106</v>
+        <v>354</v>
       </c>
       <c r="M16" s="11" t="s">
         <v>107</v>
@@ -2387,10 +2392,10 @@
         <v>109</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>348</v>
+        <v>105</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>349</v>
+        <v>106</v>
       </c>
       <c r="M17" s="11" t="s">
         <v>112</v>
@@ -2405,10 +2410,10 @@
         <v>114</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>110</v>
+        <v>348</v>
       </c>
       <c r="K18" s="7" t="s">
-        <v>111</v>
+        <v>349</v>
       </c>
       <c r="M18" s="14" t="s">
         <v>120</v>
@@ -2423,10 +2428,10 @@
         <v>118</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>346</v>
+        <v>110</v>
       </c>
       <c r="K19" s="7" t="s">
-        <v>347</v>
+        <v>111</v>
       </c>
       <c r="M19" s="15" t="s">
         <v>125</v>
@@ -2441,10 +2446,10 @@
         <v>122</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="K20" s="7" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="M20" s="15" t="s">
         <v>130</v>
@@ -3264,55 +3269,55 @@
     </row>
     <row r="110" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J110" s="7" t="s">
-        <v>324</v>
+        <v>355</v>
       </c>
       <c r="K110" s="7" t="s">
-        <v>325</v>
+        <v>227</v>
       </c>
     </row>
     <row r="111" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J111" s="7" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="K111" s="7" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="112" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J112" s="7" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="K112" s="7" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="113" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J113" s="7" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="K113" s="7" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="114" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J114" s="7" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="K114" s="7" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="115" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J115" s="7" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="K115" s="7" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="116" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J116" s="7" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="K116" s="7" t="s">
         <v>335</v>
@@ -3320,39 +3325,47 @@
     </row>
     <row r="117" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J117" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K117" s="7" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="118" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J118" s="7" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="K118" s="7" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="119" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J119" s="7" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="K119" s="7" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="120" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J120" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="K120" s="7" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="121" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J121" s="7" t="s">
         <v>343</v>
       </c>
-      <c r="K120" s="7" t="s">
+      <c r="K121" s="7" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="121" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J121" s="7"/>
-      <c r="K121" s="7" t="s">
+    <row r="122" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J122" s="7"/>
+      <c r="K122" s="7" t="s">
         <v>345</v>
       </c>
     </row>

</xml_diff>